<commit_message>
graphics and tables for final report
</commit_message>
<xml_diff>
--- a/docs/table/table_result_bm25_juris_tcu_index.xlsx
+++ b/docs/table/table_result_bm25_juris_tcu_index.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Fontes\ind-ir\docs\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28843038-3046-4BB6-9893-625BD089F83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D6EBE9-C61A-47D7-BB61-FE65DB1B843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15870" yWindow="-6015" windowWidth="15990" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -276,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -293,6 +306,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -308,14 +329,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -633,7 +647,7 @@
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,556 +664,614 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="6">
         <v>50.063000000000002</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="6">
         <v>5.48</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="7">
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="6">
         <v>51.970999999999997</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="6">
         <v>4.6100000000000003</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="9"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="6">
         <v>60.548000000000002</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="6">
         <v>3.52</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="6">
         <v>0.13500000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="6">
         <v>62.094000000000001</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="6">
         <v>3.75</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="6">
         <v>0.69299999999999995</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="6">
         <v>74.186999999999998</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="6">
         <v>2.34</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="6">
         <v>3.5000000000000003E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="10"/>
+      <c r="H6" s="19">
+        <f>C6-C5</f>
+        <v>12.092999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="18"/>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="8">
         <v>87.260999999999996</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="8">
         <v>1.48</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="8">
         <v>0.161</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="G7" s="19">
+        <f>C7-C5</f>
+        <v>25.166999999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="9">
         <v>40.082000000000001</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="9">
         <v>29.396000000000001</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="10">
         <v>0.129</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="6">
         <v>32.499000000000002</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="6">
         <v>53.042000000000002</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="11">
         <v>0.76400000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="6">
         <v>35.469000000000001</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="6">
         <v>51.615000000000002</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="11">
         <v>3.0390000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="6">
         <v>53.78</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="6">
         <v>26.905999999999999</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="11">
         <v>20.433</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="6">
         <v>48.585000000000001</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="6">
         <v>15.896000000000001</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="11">
         <v>0.77500000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="8"/>
+      <c r="H12" s="19">
+        <f>C12-C11</f>
+        <v>-5.1950000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="16"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="12">
         <v>63.506</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="12">
         <v>6.125</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="13">
         <v>3.8889999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="G13" s="19">
+        <f>C13-C11</f>
+        <v>9.7259999999999991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="9">
         <v>23.530999999999999</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="9">
         <v>53.072000000000003</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="10">
         <v>0.128</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="15"/>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="6">
         <v>22.943999999999999</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="6">
         <v>74.42</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="11">
         <v>0.79100000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="6">
         <v>26.140999999999998</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="6">
         <v>36.695999999999998</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="11">
         <v>3.0670000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="15"/>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="6">
         <v>35.299999999999997</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="6">
         <v>24.507000000000001</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="11">
         <v>20.907</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="15"/>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="6">
         <v>29.202999999999999</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="6">
         <v>14.362</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="11">
         <v>0.79900000000000004</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="8"/>
+      <c r="H18" s="19">
+        <f>C18-C17</f>
+        <v>-6.0969999999999978</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="16"/>
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="12">
         <v>46.183</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="12">
         <v>3.5219999999999998</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="13">
         <v>3.99</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="G19" s="19">
+        <f>C19-C17</f>
+        <v>10.883000000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="9">
         <v>19.34</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="9">
         <v>31.907</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="10">
         <v>0.128</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="15"/>
       <c r="B21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="6">
         <v>11.497999999999999</v>
       </c>
-      <c r="D21" s="11">
+      <c r="D21" s="6">
         <v>57.767000000000003</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E21" s="11">
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="15"/>
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="11">
+      <c r="C22" s="6">
         <v>14.09</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="6">
         <v>31.128</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="11">
         <v>3.129</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="15"/>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="11">
+      <c r="C23" s="6">
         <v>26.719000000000001</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="6">
         <v>18.384</v>
       </c>
-      <c r="E23" s="16">
+      <c r="E23" s="11">
         <v>21.216999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="15"/>
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="6">
         <v>33.853999999999999</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="6">
         <v>6.4530000000000003</v>
       </c>
-      <c r="E24" s="16">
+      <c r="E24" s="11">
         <v>0.80900000000000005</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="8"/>
+      <c r="H24" s="19">
+        <f>C24-C23</f>
+        <v>7.134999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="16"/>
       <c r="B25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="12">
         <v>43.889000000000003</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="12">
         <v>3.419</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="13">
         <v>3.8660000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="G25" s="19">
+        <f>C25-C23</f>
+        <v>17.170000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="9">
         <v>26.739000000000001</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="9">
         <v>9.1519999999999992</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="10">
         <v>0.129</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="15"/>
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="6">
         <v>23.082000000000001</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="6">
         <v>16.727</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="11">
         <v>0.79900000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="15"/>
       <c r="B28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="6">
         <v>23.091000000000001</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="6">
         <v>6.2930000000000001</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E28" s="11">
         <v>3.1179999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="15"/>
       <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="6">
         <v>37.518000000000001</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="6">
         <v>4.4749999999999996</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="11">
         <v>21.158000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="15"/>
       <c r="B30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="6">
         <v>43.710999999999999</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="6">
         <v>2.3639999999999999</v>
       </c>
-      <c r="E30" s="16">
+      <c r="E30" s="11">
         <v>0.80500000000000005</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="8"/>
+      <c r="H30" s="19">
+        <f>C30-C29</f>
+        <v>6.1929999999999978</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="16"/>
       <c r="B31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="17">
+      <c r="C31" s="12">
         <v>57.665999999999997</v>
       </c>
-      <c r="D31" s="17">
+      <c r="D31" s="12">
         <v>1.5049999999999999</v>
       </c>
-      <c r="E31" s="18">
+      <c r="E31" s="13">
         <v>4.016</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="G31" s="19">
+        <f>C31-C29</f>
+        <v>20.147999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="9">
         <v>28.326000000000001</v>
       </c>
-      <c r="D32" s="14">
+      <c r="D32" s="9">
         <v>9.6059999999999999</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="10">
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="7"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="15"/>
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="6">
         <v>24.759</v>
       </c>
-      <c r="D33" s="11">
+      <c r="D33" s="6">
         <v>16.859000000000002</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="11">
         <v>0.79800000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="15"/>
       <c r="B34" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="6">
         <v>24.555</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="6">
         <v>8.3230000000000004</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="11">
         <v>3.157</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="7"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="15"/>
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="6">
         <v>37.573</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="6">
         <v>6.899</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="11">
         <v>21.321000000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="7"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="15"/>
       <c r="B36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="6">
         <v>43.491999999999997</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="6">
         <v>2.4550000000000001</v>
       </c>
-      <c r="E36" s="16">
+      <c r="E36" s="11">
         <v>0.80600000000000005</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="8"/>
+      <c r="H36" s="19">
+        <f>C36-C35</f>
+        <v>5.9189999999999969</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="16"/>
       <c r="B37" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="12">
         <v>57.609000000000002</v>
       </c>
-      <c r="D37" s="17">
+      <c r="D37" s="12">
         <v>1.657</v>
       </c>
-      <c r="E37" s="18">
+      <c r="E37" s="13">
         <v>4.0270000000000001</v>
+      </c>
+      <c r="G37" s="19">
+        <f>C37-C35</f>
+        <v>20.036000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G39" s="19">
+        <f>AVERAGE(G7:G37)</f>
+        <v>17.188333333333333</v>
+      </c>
+      <c r="H39" s="19">
+        <f>AVERAGE(H7:H37)</f>
+        <v>1.5909999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>